<commit_message>
Dokumentáció folytatás, hiba javítás
Bug report folytatás
Autó módosítás esetén javítás
</commit_message>
<xml_diff>
--- a/Dokumentumok/BugReport.xlsx
+++ b/Dokumentumok/BugReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EKKE\GitHub\AFP_12_csop\Dokumentumok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA0334F6-1D63-42E6-ACA1-B0F89B2A0048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB2DA67-979A-42E2-98B4-D02F5896AFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5A47C97E-E1E1-434E-8D9A-E04FA1A59B98}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="105">
   <si>
     <t>IssueID</t>
   </si>
@@ -274,16 +274,105 @@
   </si>
   <si>
     <t>Megoldva / Resolved</t>
+  </si>
+  <si>
+    <t>Létrehozó, bejelentő / Creator</t>
+  </si>
+  <si>
+    <t>Osztály, Telephely esetén az azonosító módosítása nem lehet, le kellene venni a módosíthatóságot, csak a többi mező legyen módosítható.</t>
+  </si>
+  <si>
+    <t>osztalyok_lista.php, telephelyek_lista.php</t>
+  </si>
+  <si>
+    <t>Osztályok és telephelyek oldalon a kívánt soron módosítás után az azonosító módosítása mező esetén Mentés-nél  hibaüzenet (, melynek megjelenítése megmarad a lista visszatérése esetén is)</t>
+  </si>
+  <si>
+    <t>Azonosító módosítása ne legyen lehetséges, csak a többi adat</t>
+  </si>
+  <si>
+    <t>Tóth Ádám</t>
+  </si>
+  <si>
+    <t>Az előző jelenség előjön a rendszámra, mint azonosító az céges autók listájánál (az autó típusok esetén nem, mert ott a belső id nincs megjelenítve)</t>
+  </si>
+  <si>
+    <t>autok_lista.php</t>
+  </si>
+  <si>
+    <t>Hasonló, mint a BUG-002 esetén</t>
+  </si>
+  <si>
+    <t>Új elemek létrehozása (osztály, telephely, autó, autó típusok) elérhető bármilyen felhasználó részére, ha közvetlenül éri el azt. Menüsorból nem tudja elérni, csak ha esetleg tudja hogy az új autó létrehozása az uj_auto.php-ben érhető el</t>
+  </si>
+  <si>
+    <t>uj_auto.php, uj_auto_tipus.php, uj_osztaly.php, uj_telephely.php</t>
+  </si>
+  <si>
+    <t>Felhasználó tudja az oldal elérhetőségének web címét.</t>
+  </si>
+  <si>
+    <t>Be kell írni a böngészőbe az oldal elérhetőségét</t>
+  </si>
+  <si>
+    <t>Az oldal ne legyen elérhető.
+Az autok_lista.php oldal kerül betöltésre, ha nem megfelelő oldal kerül begépelésre.</t>
+  </si>
+  <si>
+    <t>Nagy Gergő</t>
+  </si>
+  <si>
+    <t>BUG-006</t>
+  </si>
+  <si>
+    <t>BUG-007</t>
+  </si>
+  <si>
+    <t>BUG-008</t>
+  </si>
+  <si>
+    <t>BUG-009</t>
+  </si>
+  <si>
+    <t>BUG-010</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>agi-kanban.vedara.net
+ oldal nem elérhető!</t>
+  </si>
+  <si>
+    <t>autok_lista.php, autok.php</t>
+  </si>
+  <si>
+    <t>A megfelelő mezők módosítása, majd mentés</t>
+  </si>
+  <si>
+    <t>Autók esetén a módosítás során a szín és beszerzés nem került mentésre.
+Valamint a rendszám (, mint azonosító) mező csak olvashatóra állítása</t>
+  </si>
+  <si>
+    <t>Rendszám mező a módosítás oldal esetén ne lehessen felülírható.
+Szín és beszezrés dátum mezők módosítása kerüljön tárolásra.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -316,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -330,6 +419,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -645,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607B9CCC-CC81-4CE0-A464-348648D58B67}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,57 +759,61 @@
     <col min="9" max="9" width="46" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="38.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" style="2" customWidth="1"/>
     <col min="13" max="13" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="2"/>
+    <col min="14" max="14" width="19.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -754,75 +853,215 @@
       <c r="M2" s="4">
         <v>45969</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O2" s="4">
         <v>45969</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="H3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="K3" s="3"/>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M3" s="4">
+        <v>45983</v>
+      </c>
+      <c r="N3" s="4"/>
+    </row>
+    <row r="4" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="K4" s="3"/>
-      <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" s="4">
+        <v>45983</v>
+      </c>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="K5" s="3"/>
-      <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M5" s="4">
+        <v>45983</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="O5" s="4">
+        <v>45984</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="B6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-      <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="L6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M6" s="4">
+        <v>45985</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M7" s="4">
+        <v>45985</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="O7" s="4">
+        <v>45985</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="3"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -831,7 +1070,11 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -840,7 +1083,11 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="3"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -849,7 +1096,11 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="3"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -858,7 +1109,7 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -867,7 +1118,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -876,7 +1127,7 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -885,7 +1136,7 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -894,7 +1145,7 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1003,6 +1254,10 @@
       <c r="K27" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="https://agi-kanban.vedara.net/" xr:uid="{A0BD634A-A8FB-4755-8935-1237B13EBBCD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>